<commit_message>
feat: Add console menu
</commit_message>
<xml_diff>
--- a/final_matrix.xlsx
+++ b/final_matrix.xlsx
@@ -429,24 +429,16 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE - 07:30AM - 11:15AM</t>
+          <t>CHAVEZ ONOFRE, CAMILA GERALDINE - 08:15AM - 05:00PM</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>HUAYANAY VELASCO, ATHINA - 11:15AM - 03:00PM</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>BARRIENTOS JERI, MILAGROS NICOL - 03:00PM - 06:45PM</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO - 07:00PM - 10:45PM</t>
-        </is>
-      </c>
+          <t>HEREDIA CAHUAYA, SUSAN NAYELLI - 05:45PM - 10:45PM</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,12 +448,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BRICEÑO LUNA, JESSICA ARACELI - 07:45AM - 06:45PM</t>
+          <t>MEZA MELO, NORMA FERNANDA - 08:30AM - 12:15PM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO - 07:00PM - 10:45PM</t>
+          <t>ZAVALA SOSA, NICOLE - 01:00PM - 10:00PM</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -475,16 +467,24 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO - 08:30AM - 12:15PM</t>
+          <t>FLORES PAREDES, LOURDES - 07:00AM - 09:45AM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ZAVALA SOSA, NICOLE - 01:00PM - 10:00PM</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+          <t>Del Aguila Murayari, Darla - 09:45AM - 01:30PM</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>VARGAS CASTRO, LOANA VICTORIA - 02:45PM - 06:30PM</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA - 07:00PM - 10:45PM</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -494,24 +494,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FLORES PAREDES, LOURDES - 07:00AM - 09:45AM</t>
+          <t>BRICEÑO LUNA, JESSICA ARACELI - 07:45AM - 06:45PM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>RUIZ SANTOS, CIELO CRISTHINA - 09:45AM - 01:30PM</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>ALTAMIZA MATOS, MERYEIN - 02:00PM - 05:45PM</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>HEREDIA CAHUAYA, SUSAN NAYELLI - 05:45PM - 10:45PM</t>
-        </is>
-      </c>
+          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO - 07:00PM - 10:45PM</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -521,7 +513,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MEZA MELO, NORMA FERNANDA - 08:30AM - 12:15PM</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO - 08:30AM - 12:15PM</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -545,7 +537,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>HUAYNATES ALTAMIRANO, JIM HANS - 03:45PM - 07:30PM</t>
+          <t>AYQUIPA MONTENEGRO, VALERIA ESTEFANY - 05:00PM - 08:45PM</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -559,14 +551,10 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CHAVEZ ONOFRE, CAMILA GERALDINE - 08:15AM - 05:00PM</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>AYALA TAPIA, DARCIE SOL - 05:00PM - 08:45PM</t>
-        </is>
-      </c>
+          <t>ERIQUE CALLE, MARIA ANTONIETA - 10:30AM - 07:15PM</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
     </row>
@@ -578,12 +566,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SUAREZ JARA, YENNIFER YUSSARA - 09:30AM - 01:15PM</t>
+          <t>BARRIENTOS JERI, MILAGROS NICOL - 03:00PM - 06:45PM</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ZEVALLOS ZANCA, VERONICA LUZ - 02:00PM - 11:00PM</t>
+          <t>CHIARA LIMA, AUGUSTO SEBASTIAN - 07:00PM - 10:45PM</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -597,19 +585,15 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ - 08:45AM - 12:30PM</t>
+          <t>DUEÑAS QUISPE, JUDYTH EVELYN - 09:00AM - 12:45PM</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>BRENIS LÁRTIGA, SEBASTIÁN - 02:00PM - 05:45PM</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN - 06:00PM - 09:45PM</t>
-        </is>
-      </c>
+          <t>ZEVALLOS ZANCA, VERONICA LUZ - 02:00PM - 11:00PM</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -620,17 +604,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DUEÑAS QUISPE, JUDYTH EVELYN - 09:00AM - 12:45PM</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE - 07:30AM - 11:15AM</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>YACILA GRANDEZ, RODRIGO ANDRE - 02:00PM - 05:45PM</t>
+          <t>SOTO VELAZCO, EMIR ALESSANDRO - 11:15AM - 03:00PM</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>LAVADO LAZARO, CELIA ELIZABETH - 06:00PM - 09:45PM</t>
+          <t>RIVERA RAZA, CATHERINE - 05:00PM - 08:45PM</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -643,17 +627,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>HUAMAN HUAMANI, ALEXIS JAVIER - 09:30AM - 01:15PM</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ - 08:45AM - 12:30PM</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>VARGAS CASTRO, LOANA VICTORIA - 02:45PM - 06:30PM</t>
+          <t>YACILA GRANDEZ, RODRIGO ANDRE - 02:00PM - 05:45PM</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CHIARA LIMA, AUGUSTO SEBASTIAN - 07:00PM - 10:45PM</t>
+          <t>NORABUENA UCHUYA, VALERIA SOFIA - 05:45PM - 09:30PM</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -666,15 +650,19 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Del Aguila Murayari, Darla - 09:45AM - 01:30PM</t>
+          <t>HUAMAN HUAMANI, ALEXIS JAVIER - 09:30AM - 01:15PM</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>AYQUIPA MONTENEGRO, VALERIA ESTEFANY - 05:00PM - 08:45PM</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
+          <t>ALTAMIZA MATOS, MERYEIN - 02:00PM - 05:45PM</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN - 06:00PM - 09:45PM</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
@@ -685,15 +673,19 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>VEGA RIVAS, ANDREA FERNANDA - 10:00AM - 01:45PM</t>
+          <t>SUAREZ JARA, YENNIFER YUSSARA - 09:30AM - 01:15PM</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CORDOVA MONTALVO, MELANY KARINA - 05:00PM - 08:45PM</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
+          <t>BRENIS LÁRTIGA, SEBASTIÁN - 02:00PM - 05:45PM</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>LAVADO LAZARO, CELIA ELIZABETH - 06:00PM - 09:45PM</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -704,12 +696,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MEZA PEREZ, JUAN CRISTOFER - 10:00AM - 01:45PM</t>
+          <t>RUIZ SANTOS, CIELO CRISTHINA - 09:45AM - 01:30PM</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>RIVERA RAZA, CATHERINE - 05:00PM - 08:45PM</t>
+          <t>HUAYNATES ALTAMIRANO, JIM HANS - 03:45PM - 07:30PM</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -723,12 +715,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MUÑANTE MONDRAGÓN, MATIAS SEBÁSTIAN - 10:15AM - 02:00PM</t>
+          <t>VEGA RIVAS, ANDREA FERNANDA - 10:00AM - 01:45PM</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>NORABUENA UCHUYA, VALERIA SOFIA - 05:45PM - 09:30PM</t>
+          <t>AYALA TAPIA, DARCIE SOL - 05:00PM - 08:45PM</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>

</xml_diff>

<commit_message>
implement read pdf feature
</commit_message>
<xml_diff>
--- a/final_matrix.xlsx
+++ b/final_matrix.xlsx
@@ -429,12 +429,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>CHAVEZ ONOFRE, CAMILA GERALDINE - 08:15AM - 05:00PM</t>
+          <t>BRICEÑO LUNA , JESSICA ARACELI - 06:30AM - 05:30PM</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>HEREDIA CAHUAYA, SUSAN NAYELLI - 05:45PM - 10:45PM</t>
+          <t>MEDINA MARCELO, NAOMI ARIADNA - 05:30PM - 09:15PM</t>
         </is>
       </c>
       <c r="D1" t="inlineStr"/>
@@ -448,12 +448,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MEZA MELO, NORMA FERNANDA - 08:30AM - 12:15PM</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ - 08:30AM - 12:15PM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ZAVALA SOSA, NICOLE - 01:00PM - 10:00PM</t>
+          <t>SOTELO GONZALES , CAMILA SOFÍA - 01:00PM - 10:00PM</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -467,24 +467,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FLORES PAREDES, LOURDES - 07:00AM - 09:45AM</t>
+          <t>QUISPE MONDRAGÓN , JUAN ALFONSO - 09:15AM - 01:00PM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Del Aguila Murayari, Darla - 09:45AM - 01:30PM</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>VARGAS CASTRO, LOANA VICTORIA - 02:45PM - 06:30PM</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA - 07:00PM - 10:45PM</t>
-        </is>
-      </c>
+          <t>BARRIENTOS JERI, MILAGROS NICOL - 01:45PM - 10:45PM</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -494,16 +486,24 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BRICEÑO LUNA, JESSICA ARACELI - 07:45AM - 06:45PM</t>
+          <t>MONTEZUMA DEJO, EVELYN BRUNELLA - 07:00AM - 10:45AM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO - 07:00PM - 10:45PM</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+          <t>YOVERA ROBLES, VICTOR EDUARDO - 10:45AM - 02:30PM</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>INGA DELGADO, CARLOS DANIEL - 03:00PM - 06:45PM</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>BRENIS LÁRTIGA , SEBASTIÁN - 07:00PM - 10:45PM</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -513,12 +513,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO - 08:30AM - 12:15PM</t>
+          <t>MARTINEZ PAZ, ROCIO ESPERANZA - 09:00AM - 06:00PM</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>TITO LAURA, NANCY FIORELLA - 12:30PM - 09:30PM</t>
+          <t>SALAS VILLANUEVA, JAMILA DASHA - 06:00PM - 09:45PM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -532,15 +532,19 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>HUAMANI TORRES, LUIS RODRIGO - 06:30AM - 03:15PM</t>
+          <t>POBLETE SAIRE, FIORELLA ESTHER - 07:30AM - 11:15AM</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>AYQUIPA MONTENEGRO, VALERIA ESTEFANY - 05:00PM - 08:45PM</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL - 11:15AM - 03:00PM</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>RIVERA CARREÑO , DIANA DESIRÉE - 03:30PM - 07:15PM</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
@@ -551,11 +555,19 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ERIQUE CALLE, MARIA ANTONIETA - 10:30AM - 07:15PM</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+          <t>ALVITE CORNEJO, ANGIE LUCERO - 07:30AM - 11:15AM</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CUSI QUISPE, ANDREA ESTEFANY - 11:15AM - 03:00PM</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>HUAYNATES ALTAMIRANO, JIM HANS - 04:00PM - 07:45PM</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -566,15 +578,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BARRIENTOS JERI, MILAGROS NICOL - 03:00PM - 06:45PM</t>
+          <t>MEZA PEREZ, JUAN CRISTOFER - 09:15AM - 01:00PM</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CHIARA LIMA, AUGUSTO SEBASTIAN - 07:00PM - 10:45PM</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
+          <t>YACILA GRANDEZ, RODRIGO ANDRE - 02:00PM - 05:45PM</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>YANAC DAVILA, GERALD RONNY - 05:45PM - 09:30PM</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -585,15 +601,19 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DUEÑAS QUISPE, JUDYTH EVELYN - 09:00AM - 12:45PM</t>
+          <t>MORENO CANCHANYA, ROSMERY - 10:15AM - 02:00PM</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ZEVALLOS ZANCA, VERONICA LUZ - 02:00PM - 11:00PM</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
+          <t>PARICELA TINEO, JAIME DANIEL - 02:00PM - 05:45PM</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>MENDOZA DIEGO, ZAIDA VANESSA - 06:00PM - 09:45PM</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -604,17 +624,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE - 07:30AM - 11:15AM</t>
+          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO - 10:15AM - 02:00PM</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>SOTO VELAZCO, EMIR ALESSANDRO - 11:15AM - 03:00PM</t>
+          <t>VARGAS CASTRO, LOANA VICTORIA - 02:00PM - 05:45PM</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>RIVERA RAZA, CATHERINE - 05:00PM - 08:45PM</t>
+          <t>FLORES PAREDES, LOURDES - 06:00PM - 08:45PM</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -627,19 +647,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ - 08:45AM - 12:30PM</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>YACILA GRANDEZ, RODRIGO ANDRE - 02:00PM - 05:45PM</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>NORABUENA UCHUYA, VALERIA SOFIA - 05:45PM - 09:30PM</t>
-        </is>
-      </c>
+          <t>ZAVALA SOSA, NICOLE - 11:00AM - 08:00PM</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -650,19 +662,15 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>HUAMAN HUAMANI, ALEXIS JAVIER - 09:30AM - 01:15PM</t>
+          <t>AYALA MORA, CECILIA ROSARIO - 10:30AM - 02:15PM</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ALTAMIZA MATOS, MERYEIN - 02:00PM - 05:45PM</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>CARDENAS RICAPA, FABRIZIO ESTEBAN - 06:00PM - 09:45PM</t>
-        </is>
-      </c>
+          <t>VILCHEZ CUBA, JACK ANTHONY - 04:15PM - 08:00PM</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
@@ -673,19 +681,15 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SUAREZ JARA, YENNIFER YUSSARA - 09:30AM - 01:15PM</t>
+          <t>GOMEZ ALBINO, IDALIA GIMENA - 11:15AM - 03:00PM</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>BRENIS LÁRTIGA, SEBASTIÁN - 02:00PM - 05:45PM</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>LAVADO LAZARO, CELIA ELIZABETH - 06:00PM - 09:45PM</t>
-        </is>
-      </c>
+          <t>ARIAS MACHACUAY, SADELITH SORAGGI - 04:30PM - 08:15PM</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -696,12 +700,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>RUIZ SANTOS, CIELO CRISTHINA - 09:45AM - 01:30PM</t>
+          <t>HUAMAN HUAMANI, ALEXIS JAVIER - 11:15AM - 03:00PM</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HUAYNATES ALTAMIRANO, JIM HANS - 03:45PM - 07:30PM</t>
+          <t>MENDOZA CRUZ, LILIANA LILIANA - 04:45PM - 08:30PM</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -715,12 +719,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>VEGA RIVAS, ANDREA FERNANDA - 10:00AM - 01:45PM</t>
+          <t>HUAYANAY VELASCO, ATHINA - 11:15AM - 03:00PM</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>AYALA TAPIA, DARCIE SOL - 05:00PM - 08:45PM</t>
+          <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO - 05:30PM - 09:15PM</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>

</xml_diff>

<commit_message>
chore: Refactor code to improve readability and handle empty day schedule
</commit_message>
<xml_diff>
--- a/final_matrix.xlsx
+++ b/final_matrix.xlsx
@@ -429,12 +429,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>BRICEÑO LUNA , JESSICA ARACELI - 06:30AM - 05:30PM</t>
+          <t>VEGA CARDENAS, ANGELICA LOURDES - 08:15AM - 12:00PM</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>MEDINA MARCELO, NAOMI ARIADNA - 05:30PM - 09:15PM</t>
+          <t>SOTELO GONZALES, CAMILA SOFÍA - 01:30PM - 10:30PM</t>
         </is>
       </c>
       <c r="D1" t="inlineStr"/>
@@ -448,12 +448,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ - 08:30AM - 12:15PM</t>
+          <t>MARTINEZ PAZ, ROCIO ESPERANZA - 08:45AM - 05:45PM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SOTELO GONZALES , CAMILA SOFÍA - 01:00PM - 10:00PM</t>
+          <t>SALAS VILLANUEVA, JAMILA DASHA - 05:45PM - 09:30PM</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -467,12 +467,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGÓN , JUAN ALFONSO - 09:15AM - 01:00PM</t>
+          <t>POBLETE SAIRE, FIORELLA ESTHER - 09:15AM - 01:00PM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BARRIENTOS JERI, MILAGROS NICOL - 01:45PM - 10:45PM</t>
+          <t>TITO LAURA, NANCY FIORELLA - 02:00PM - 11:00PM</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -486,22 +486,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MONTEZUMA DEJO, EVELYN BRUNELLA - 07:00AM - 10:45AM</t>
+          <t>YOVERA ROBLES, VICTOR EDUARDO - 06:30AM - 10:15AM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>YOVERA ROBLES, VICTOR EDUARDO - 10:45AM - 02:30PM</t>
+          <t>MONTEZUMA DEJO, EVELYN BRUNELLA - 10:15AM - 02:00PM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>INGA DELGADO, CARLOS DANIEL - 03:00PM - 06:45PM</t>
+          <t>PARICELA TINEO, JAIME DANIEL - 02:00PM - 05:45PM</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>BRENIS LÁRTIGA , SEBASTIÁN - 07:00PM - 10:45PM</t>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN - 06:00PM - 09:45PM</t>
         </is>
       </c>
     </row>
@@ -513,15 +513,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MARTINEZ PAZ, ROCIO ESPERANZA - 09:00AM - 06:00PM</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO - 07:00AM - 10:45AM</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SALAS VILLANUEVA, JAMILA DASHA - 06:00PM - 09:45PM</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+          <t>RUIZ SANTOS, CIELO CRISTHINA - 11:00AM - 02:45PM</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>RIVERA CARREÑO, DIANA DESIRÉE - 03:30PM - 07:15PM</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -532,17 +536,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>POBLETE SAIRE, FIORELLA ESTHER - 07:30AM - 11:15AM</t>
+          <t>HUAMAN HUAMANI, ALEXIS JAVIER - 08:30AM - 12:15PM</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CARHUARICRA ESPINOZA, FIORELLA NICOLL - 11:15AM - 03:00PM</t>
+          <t>CAPCHA YARANGO, DAVID - 02:00PM - 05:45PM</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>RIVERA CARREÑO , DIANA DESIRÉE - 03:30PM - 07:15PM</t>
+          <t>ARIAS MACHACUAY, SADELITH SORAGGI - 05:45PM - 09:30PM</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -555,17 +559,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO - 07:30AM - 11:15AM</t>
+          <t>QUISPE MONDRAGÓN, JUAN ALFONSO - 08:00AM - 11:45AM</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CUSI QUISPE, ANDREA ESTEFANY - 11:15AM - 03:00PM</t>
+          <t>BARRIENTOS JERI, MILAGROS NICOL - 12:00PM - 03:30PM</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>HUAYNATES ALTAMIRANO, JIM HANS - 04:00PM - 07:45PM</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL - 03:30PM - 07:15PM</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -578,19 +582,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MEZA PEREZ, JUAN CRISTOFER - 09:15AM - 01:00PM</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>YACILA GRANDEZ, RODRIGO ANDRE - 02:00PM - 05:45PM</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>YANAC DAVILA, GERALD RONNY - 05:45PM - 09:30PM</t>
-        </is>
-      </c>
+          <t>BRICEÑO LUNA, JESSICA ARACELI - 11:00AM - 10:00PM</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -601,17 +597,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MORENO CANCHANYA, ROSMERY - 10:15AM - 02:00PM</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ - 09:00AM - 12:45PM</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>PARICELA TINEO, JAIME DANIEL - 02:00PM - 05:45PM</t>
+          <t>YACILA GRANDEZ, RODRIGO ANDRE - 02:00PM - 05:45PM</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>MENDOZA DIEGO, ZAIDA VANESSA - 06:00PM - 09:45PM</t>
+          <t>FLORES PAREDES, LOURDES - 06:00PM - 08:45PM</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -624,19 +620,15 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO - 10:15AM - 02:00PM</t>
+          <t>AYALA MORA, CECILIA ROSARIO - 11:15AM - 03:00PM</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>VARGAS CASTRO, LOANA VICTORIA - 02:00PM - 05:45PM</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>FLORES PAREDES, LOURDES - 06:00PM - 08:45PM</t>
-        </is>
-      </c>
+          <t>CHAVEZ ONOFRE, CAMILA GERALDINE - 06:00PM - 10:30PM</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -647,10 +639,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ZAVALA SOSA, NICOLE - 11:00AM - 08:00PM</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
+          <t>MEZA PEREZ, JUAN CRISTOFER - 09:15AM - 01:00PM</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>BONILLA SÁNCHEZ, RAÚL FERNANDO - 03:45PM - 07:30PM</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
     </row>
@@ -662,12 +658,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AYALA MORA, CECILIA ROSARIO - 10:30AM - 02:15PM</t>
+          <t>HUAYANAY VELASCO, ATHINA - 10:00AM - 01:45PM</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>VILCHEZ CUBA, JACK ANTHONY - 04:15PM - 08:00PM</t>
+          <t>MENDOZA CRUZ, LILIANA LILIANA - 04:30PM - 08:15PM</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -681,12 +677,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>GOMEZ ALBINO, IDALIA GIMENA - 11:15AM - 03:00PM</t>
+          <t>GOMEZ ALBINO, IDALIA GIMENA - 10:15AM - 02:00PM</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ARIAS MACHACUAY, SADELITH SORAGGI - 04:30PM - 08:15PM</t>
+          <t>MEDINA MARCELO, NAOMI ARIADNA - 04:30PM - 08:15PM</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -700,12 +696,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>HUAMAN HUAMANI, ALEXIS JAVIER - 11:15AM - 03:00PM</t>
+          <t>ILDEFONSO MOTTA, JHOSSEP ANGELO - 10:15AM - 02:00PM</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MENDOZA CRUZ, LILIANA LILIANA - 04:45PM - 08:30PM</t>
+          <t>MENDOZA DIEGO, ZAIDA VANESSA - 05:15PM - 09:00PM</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -719,12 +715,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>HUAYANAY VELASCO, ATHINA - 11:15AM - 03:00PM</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE - 11:15AM - 03:00PM</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>TORRES RAZURI, JESUS GUSTAVO SANTIAGO - 05:30PM - 09:15PM</t>
+          <t>SUAREZ JARA, YENNIFER YUSSARA - 05:30PM - 09:15PM</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>

</xml_diff>